<commit_message>
feat(exportFile): Fix code smell generate excel file
</commit_message>
<xml_diff>
--- a/export.xlsx
+++ b/export.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="27">
   <si>
     <t>Shop:</t>
   </si>
@@ -53,7 +53,7 @@
     <t/>
   </si>
   <si>
-    <t>Shop Note</t>
+    <t>Shop Note:</t>
   </si>
   <si>
     <t>ARTICLE_NUMBER</t>
@@ -123,8 +123,8 @@
     <font>
       <name val="Arial"/>
       <sz val="10.0"/>
+      <color indexed="12"/>
       <b val="true"/>
-      <color indexed="12"/>
     </font>
   </fonts>
   <fills count="7">
@@ -159,7 +159,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -168,16 +168,16 @@
       <diagonal/>
     </border>
     <border>
-      <right style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
     <border>
       <left style="thin"/>
-      <right style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
       <top style="thin"/>
+      <bottom style="thin"/>
     </border>
     <border>
       <left style="thin"/>
@@ -186,21 +186,6 @@
       <bottom style="thin"/>
     </border>
     <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
       <bottom style="thin">
         <color indexed="8"/>
       </bottom>
@@ -286,26 +271,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="true" applyFill="true" applyAlignment="true" applyBorder="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyAlignment="true" applyFont="true">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment horizontal="left" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyBorder="true" applyAlignment="true" applyFont="true">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyBorder="true" applyFont="true" applyAlignment="true">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyFill="true" applyAlignment="true">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyAlignment="true" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyAlignment="true" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyAlignment="true" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -334,112 +318,114 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" t="s" s="4">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="n">
+      <c r="B1" t="n" s="3">
         <v>4.0</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="4" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="6"/>
+      <c r="G1" t="s" s="4">
         <v>1</v>
       </c>
-      <c r="H1" s="7"/>
-      <c r="I1" s="3" t="s">
+      <c r="H1" s="6"/>
+      <c r="I1" t="s" s="3">
         <v>2</v>
       </c>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="7"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="6"/>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" t="s" s="4">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="n">
+      <c r="B2" t="n" s="3">
         <v>5.0</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="4" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="6"/>
+      <c r="G2" t="s" s="4">
         <v>4</v>
       </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="3" t="s">
+      <c r="H2" s="6"/>
+      <c r="I2" t="s" s="3">
         <v>5</v>
       </c>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="7"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="6"/>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" t="s" s="4">
         <v>6</v>
       </c>
-      <c r="B3" s="3" t="n">
+      <c r="B3" t="n" s="3">
         <v>9.0</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="4" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="6"/>
+      <c r="G3" t="s" s="4">
         <v>7</v>
       </c>
-      <c r="H3" s="7"/>
-      <c r="I3" s="3" t="s">
+      <c r="H3" s="6"/>
+      <c r="I3" t="s" s="3">
         <v>8</v>
       </c>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="7"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="6"/>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="s">
+      <c r="A4" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="B4" s="3" t="n">
+      <c r="B4" t="n" s="3">
         <v>7.0</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="4" t="s">
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="6"/>
+      <c r="G4" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="H4" s="7"/>
-      <c r="I4" s="3" t="s">
+      <c r="H4" s="6"/>
+      <c r="I4" t="s" s="3">
         <v>11</v>
       </c>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="7"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="6"/>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="4" t="s">
+      <c r="A5" t="s" s="4">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s" s="3">
+        <v>12</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="6"/>
+      <c r="G5" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="H5" s="7"/>
-      <c r="I5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="7"/>
+      <c r="H5" s="6"/>
+      <c r="I5" t="s" s="3">
+        <v>12</v>
+      </c>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="6"/>
     </row>
     <row r="6">
       <c r="A6" t="s" s="1">
@@ -473,9 +459,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" s="2" customFormat="true">
+    <row r="7">
       <c r="A7" t="n" s="2">
-        <v>1.27395199E8</v>
+        <v>1.2739519E8</v>
       </c>
       <c r="B7" t="n" s="2">
         <v>1373.0</v>
@@ -505,7 +491,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" s="2" customFormat="true">
+    <row r="8">
       <c r="A8" t="n" s="2">
         <v>1.43478032E8</v>
       </c>
@@ -537,7 +523,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" s="2" customFormat="true">
+    <row r="9">
       <c r="A9" t="n" s="2">
         <v>1.11946224E8</v>
       </c>
@@ -569,7 +555,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" s="2" customFormat="true">
+    <row r="10">
       <c r="A10" t="n" s="2">
         <v>1.11946277E8</v>
       </c>
@@ -601,7 +587,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" s="2" customFormat="true">
+    <row r="11">
       <c r="A11" t="n" s="2">
         <v>1.25778255E8</v>
       </c>
@@ -633,7 +619,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" s="2" customFormat="true">
+    <row r="12">
       <c r="A12" t="n" s="2">
         <v>1.34025711E8</v>
       </c>
@@ -665,7 +651,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" s="2" customFormat="true">
+    <row r="13">
       <c r="A13" t="n" s="2">
         <v>1.47812747E8</v>
       </c>

</xml_diff>